<commit_message>
reorganizacion de carpetas y archivos
</commit_message>
<xml_diff>
--- a/usuarios/facundo.xlsx
+++ b/usuarios/facundo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\comedores_unr\usuarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1BDDC53-16D0-4BCF-9CC8-42EFFF9117BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96C3575-AFDA-4500-AC84-4796AC76829E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{5C91FBF1-797B-4D74-8CDC-7038822E3838}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
   <si>
     <t>comedor</t>
   </si>
@@ -333,27 +333,27 @@
       <sheetData sheetId="5">
         <row r="2">
           <cell r="A2">
-            <v>45817</v>
+            <v>45831</v>
           </cell>
         </row>
         <row r="3">
           <cell r="A3">
-            <v>45818</v>
+            <v>45832</v>
           </cell>
         </row>
         <row r="4">
           <cell r="A4">
-            <v>45819</v>
+            <v>45833</v>
           </cell>
         </row>
         <row r="5">
           <cell r="A5">
-            <v>45820</v>
+            <v>45834</v>
           </cell>
         </row>
         <row r="6">
           <cell r="A6">
-            <v>45821</v>
+            <v>45835</v>
           </cell>
         </row>
       </sheetData>
@@ -678,7 +678,7 @@
   <dimension ref="A1:C747"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -705,10 +705,65 @@
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C2" s="7">
-        <v>45817</v>
+        <v>45831</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="7">
+        <v>45832</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="7">
+        <v>45833</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7">
+        <v>45833</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="7">
+        <v>45834</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="7">
+        <v>45835</v>
       </c>
     </row>
     <row r="17" spans="3:3" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2986,21 +3041,21 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>COUNTA(Table1[comedor])</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" s="8">
         <v>1500</v>
       </c>
       <c r="C2" s="8">
         <f>A2*B2</f>
-        <v>1500</v>
+        <v>9000</v>
       </c>
       <c r="D2" s="8">
         <v>6400</v>
       </c>
       <c r="E2" s="8">
         <f>C2-D2</f>
-        <v>-4900</v>
+        <v>2600</v>
       </c>
     </row>
   </sheetData>
@@ -3332,31 +3387,31 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>45817</v>
+        <v>45831</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>45818</v>
+        <v>45832</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>45819</v>
+        <v>45833</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>45820</v>
+        <v>45834</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>45821</v>
+        <v>45835</v>
       </c>
       <c r="C6" s="2"/>
     </row>

</xml_diff>

<commit_message>
cambio en la gestion del swal-container para acelerar la confirmacion del menú
</commit_message>
<xml_diff>
--- a/usuarios/facundo.xlsx
+++ b/usuarios/facundo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\comedores_unr\usuarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74127265-E7E2-4C31-BE81-0B35CD8A2A9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FB2CA7-AE5C-4E20-BAF3-204223C36E4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{5C91FBF1-797B-4D74-8CDC-7038822E3838}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
   <si>
     <t>comedor</t>
   </si>
@@ -363,8 +363,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F0EF193-EB81-4522-8735-E94CBF699BB1}" name="Table1" displayName="Table1" ref="A1:C1048575" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C1048575" xr:uid="{0CB89399-0A52-40D9-808D-F0E65FB1840C}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F0EF193-EB81-4522-8735-E94CBF699BB1}" name="Table1" displayName="Table1" ref="A1:C1048571" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C1048571" xr:uid="{0CB89399-0A52-40D9-808D-F0E65FB1840C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -675,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E57EADAA-D27F-4196-9F5D-6F9B5C2B1711}">
-  <dimension ref="A1:C746"/>
+  <dimension ref="A1:C742"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -708,52 +708,24 @@
         <v>17</v>
       </c>
       <c r="C2" s="7">
-        <v>45873</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="7">
-        <v>45874</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="7">
-        <v>45875</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="7">
-        <v>45876</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="7">
         <v>45877</v>
       </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
@@ -3663,34 +3635,18 @@
       <c r="A742" s="5"/>
       <c r="B742" s="5"/>
     </row>
-    <row r="743" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A743" s="5"/>
-      <c r="B743" s="5"/>
-    </row>
-    <row r="744" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A744" s="5"/>
-      <c r="B744" s="5"/>
-    </row>
-    <row r="745" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A745" s="5"/>
-      <c r="B745" s="5"/>
-    </row>
-    <row r="746" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A746" s="5"/>
-      <c r="B746" s="5"/>
-    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B857:B1048576" xr:uid="{531AE5A0-EC89-48F8-A3E5-33FE2ABF0ED1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B853:B1048576" xr:uid="{531AE5A0-EC89-48F8-A3E5-33FE2ABF0ED1}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048575" xr:uid="{10A41909-0E0A-4314-8207-4DA0B7C8508D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048571" xr:uid="{10A41909-0E0A-4314-8207-4DA0B7C8508D}">
       <formula1>comedores</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B856" xr:uid="{16E48105-2273-4AEA-A8CC-0B45FAF705D5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B852" xr:uid="{16E48105-2273-4AEA-A8CC-0B45FAF705D5}">
       <formula1>INDIRECT(A2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C746" xr:uid="{E0DE0EAF-91D8-4659-A19F-B68973C47013}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C742" xr:uid="{E0DE0EAF-91D8-4659-A19F-B68973C47013}">
       <formula1>fechas</formula1>
     </dataValidation>
   </dataValidations>
@@ -3704,12 +3660,12 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F3F5093F-5F34-4818-8517-C09E64BC83B2}">
           <x14:formula1>
-            <xm:f>fechas!A746</xm:f>
+            <xm:f>fechas!A742</xm:f>
           </x14:formula1>
           <x14:formula2>
             <xm:f>fechas!#REF!</xm:f>
           </x14:formula2>
-          <xm:sqref>C747:C1048576</xm:sqref>
+          <xm:sqref>C743:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3750,21 +3706,21 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>COUNTA(Table1[comedor])</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" s="8">
         <v>1500</v>
       </c>
       <c r="C2" s="8">
         <f>A2*B2</f>
-        <v>7500</v>
+        <v>1500</v>
       </c>
       <c r="D2" s="8">
         <v>6400</v>
       </c>
       <c r="E2" s="8">
         <f>C2-D2</f>
-        <v>1100</v>
+        <v>-4900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
funcionalidad para finalizar la ejecucion del script
</commit_message>
<xml_diff>
--- a/usuarios/facundo.xlsx
+++ b/usuarios/facundo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\comedores_unr\usuarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FB2CA7-AE5C-4E20-BAF3-204223C36E4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80AF6F7-9226-407C-9D80-2F66AB85AE8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{5C91FBF1-797B-4D74-8CDC-7038822E3838}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="35">
   <si>
     <t>comedor</t>
   </si>
@@ -678,7 +678,7 @@
   <dimension ref="A1:C742"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,51 @@
         <v>17</v>
       </c>
       <c r="C2" s="7">
-        <v>45877</v>
+        <v>45880</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="7">
+        <v>45881</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="7">
+        <v>45882</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7">
+        <v>45883</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7">
+        <v>45884</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3706,21 +3750,21 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>COUNTA(Table1[comedor])</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B2" s="8">
         <v>1500</v>
       </c>
       <c r="C2" s="8">
         <f>A2*B2</f>
-        <v>1500</v>
+        <v>7500</v>
       </c>
       <c r="D2" s="8">
         <v>6400</v>
       </c>
       <c r="E2" s="8">
         <f>C2-D2</f>
-        <v>-4900</v>
+        <v>1100</v>
       </c>
     </row>
   </sheetData>
@@ -4036,7 +4080,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4052,31 +4096,31 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>45873</v>
+        <v>45880</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>45874</v>
+        <v>45881</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>45875</v>
+        <v>45882</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>45876</v>
+        <v>45883</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>45877</v>
+        <v>45884</v>
       </c>
       <c r="C6" s="2"/>
     </row>

</xml_diff>

<commit_message>
funcion cargar credito:redireccionamiento mercado pago
</commit_message>
<xml_diff>
--- a/usuarios/facundo.xlsx
+++ b/usuarios/facundo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\comedores_unr\usuarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80AF6F7-9226-407C-9D80-2F66AB85AE8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7349AF16-5E89-4DF1-A2D7-89F74412B1A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{5C91FBF1-797B-4D74-8CDC-7038822E3838}"/>
   </bookViews>
@@ -678,7 +678,7 @@
   <dimension ref="A1:C742"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="7">
-        <v>45880</v>
+        <v>45887</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -716,10 +716,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="7">
-        <v>45881</v>
+        <v>45888</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -727,10 +727,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C4" s="7">
-        <v>45882</v>
+        <v>45889</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -741,7 +741,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="7">
-        <v>45883</v>
+        <v>45890</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -752,7 +752,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="7">
-        <v>45884</v>
+        <v>45891</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4080,7 +4080,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="C2" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4096,31 +4096,31 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>45880</v>
+        <v>45887</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>45881</v>
+        <v>45888</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>45882</v>
+        <v>45889</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>45883</v>
+        <v>45890</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>45884</v>
+        <v>45891</v>
       </c>
       <c r="C6" s="2"/>
     </row>

</xml_diff>